<commit_message>
<faster loading app but callback error present but still working>
</commit_message>
<xml_diff>
--- a/bess_data.xlsx
+++ b/bess_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\QT 2025\BESS Failure\Git Excel Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{924EF221-D7F1-4DB1-94DF-95C36A4C7F05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA852B1B-C4F3-42B9-B385-ED6071790C04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{28A21EE0-A8E3-4C26-8939-9CC42DC6429D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1033" uniqueCount="569">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1034" uniqueCount="570">
   <si>
     <t>Location</t>
   </si>
@@ -1752,6 +1752,9 @@
   </si>
   <si>
     <t>Long</t>
+  </si>
+  <si>
+    <t>https://www.staradvertiser.com/wp-content/uploads/2015/11/20120801_brk_windfarmmap.jpg</t>
   </si>
 </sst>
 </file>
@@ -2118,10 +2121,10 @@
   <dimension ref="A1:AC95"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="R2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="Y2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="S2" sqref="S2"/>
+      <selection pane="bottomRight" activeCell="Y3" sqref="Y3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2334,6 +2337,9 @@
       <c r="X3" t="s">
         <v>43</v>
       </c>
+      <c r="Y3" t="s">
+        <v>569</v>
+      </c>
       <c r="AB3" t="s">
         <v>557</v>
       </c>

</xml_diff>

<commit_message>
<bess_data.xlsx updated to correcty Wyoming>
</commit_message>
<xml_diff>
--- a/bess_data.xlsx
+++ b/bess_data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\QT 2025\BESS Failure\Git Excel Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\QT 2025\BESS Failure\Git Excel Files\Git commit update\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA852B1B-C4F3-42B9-B385-ED6071790C04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1B200978-1682-4DE8-A640-34A976E9DCEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{28A21EE0-A8E3-4C26-8939-9CC42DC6429D}"/>
   </bookViews>
@@ -2121,10 +2121,10 @@
   <dimension ref="A1:AC95"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="Y2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="S2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Y3" sqref="Y3"/>
+      <selection pane="bottomRight" activeCell="S65" sqref="S65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5330,7 +5330,7 @@
         <v>44.427999999999997</v>
       </c>
       <c r="S65" s="4">
-        <v>110.5885</v>
+        <v>-110.5885</v>
       </c>
       <c r="V65" t="s">
         <v>375</v>

</xml_diff>